<commit_message>
update template excel server side
</commit_message>
<xml_diff>
--- a/server/assets/template_ropa.xlsx
+++ b/server/assets/template_ropa.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1FA02B-0F83-AF42-96BB-4E36A9B39E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E32C94-EBE7-694E-9060-DBB9584A2BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t xml:space="preserve">แบบบันทึกรายการตามมาตรา 39 (Record of Processing Activity) </t>
   </si>
@@ -248,9 +248,6 @@
     <t xml:space="preserve">ชื่อผู้ควบคุมข้อมูลส่วนบุคคล (หรือผู้แทน) </t>
   </si>
   <si>
-    <t>Siriram Hazam</t>
-  </si>
-  <si>
     <t xml:space="preserve">ชื่อเจ้าหน้าที่คุ้มครองข้อมูลส่วนบุคคล </t>
   </si>
   <si>
@@ -270,9 +267,6 @@
   </si>
   <si>
     <t>หน่วยงานที่บันทึกรายการ</t>
-  </si>
-  <si>
-    <t>test123</t>
   </si>
   <si>
     <t>กิจกรรมงานที่บันทึกรายการ</t>
@@ -287,15 +281,6 @@
   </si>
   <si>
     <t>ได้รับข้อมูลมาจาก</t>
-  </si>
-  <si>
-    <t>รูปแบบของข้อมูล 
-(ข้อมูลทั่วไป/
-ข้อมูลอ่อนไหว)</t>
-  </si>
-  <si>
-    <t>ประเภทของข้อมูลส่วนบุคคล
-(กลุ่มของข้อมูล )</t>
   </si>
   <si>
     <t>วัตถุประสงค์ของการเก็บรวบรวมข้อมูล (แยกระบุวัตถุประสงค์ตามประเภทข้อมูล</t>
@@ -393,6 +378,14 @@
   </si>
   <si>
     <t>เงื่อนไขในการเข้าถึงข้อมูล</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ประเภทของข้อมูลส่วนบุคคล (ข้อมูลทั่วไป/
+ข้อมูลอ่อนไหว)</t>
+  </si>
+  <si>
+    <t>รูปแบบของข้อมูลส่วนบุคคล
+(กลุ่มของข้อมูล )</t>
   </si>
 </sst>
 </file>
@@ -830,6 +823,69 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -848,74 +904,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1253,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1277,264 +1270,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="18"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="39"/>
     </row>
     <row r="3" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="21"/>
+        <v>3</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="22"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="41"/>
     </row>
     <row r="4" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
+        <v>4</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="30"/>
     </row>
     <row r="5" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="27"/>
+        <v>5</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="31"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="33"/>
     </row>
     <row r="6" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="28"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
+        <v>8</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="25"/>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="32"/>
+        <v>9</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="27"/>
     </row>
     <row r="9" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="D9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="G9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="H9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="I9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="J9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="O9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="P9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="33" t="s">
+      <c r="Q9" s="15" t="s">
         <v>21</v>
-      </c>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q9" s="40" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="41"/>
+        <v>25</v>
+      </c>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="1:17" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
@@ -1609,22 +1594,13 @@
     <row r="27" ht="17" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:Q2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:Q3"/>
     <mergeCell ref="K6:Q6"/>
     <mergeCell ref="B7:Q7"/>
     <mergeCell ref="B8:Q8"/>
@@ -1634,13 +1610,22 @@
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:Q2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="J9:M9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
DPO and Activities Status in Excel Done
</commit_message>
<xml_diff>
--- a/server/assets/template_ropa.xlsx
+++ b/server/assets/template_ropa.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E32C94-EBE7-694E-9060-DBB9584A2BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EE97D5-0FCE-384D-B458-A3A1CA42C326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36400" yWindow="1980" windowWidth="28820" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,15 +240,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t xml:space="preserve">แบบบันทึกรายการตามมาตรา 39 (Record of Processing Activity) </t>
   </si>
   <si>
     <t xml:space="preserve">ชื่อผู้ควบคุมข้อมูลส่วนบุคคล (หรือผู้แทน) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ชื่อเจ้าหน้าที่คุ้มครองข้อมูลส่วนบุคคล </t>
   </si>
   <si>
     <t>ที่ตั้งของสถานที่ติดต่อ</t>
@@ -387,12 +384,18 @@
     <t>รูปแบบของข้อมูลส่วนบุคคล
 (กลุ่มของข้อมูล )</t>
   </si>
+  <si>
+    <t>ชื่อเจ้าหน้าที่คุ้มครองข้อมูลส่วนบุคคล (DPO)</t>
+  </si>
+  <si>
+    <t>สถานะของการตรวจสอบ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,21 +430,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="TH SarabunPSK"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
-      <name val="TH SarabunPSK"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
       <name val="TH SarabunPSK"/>
       <family val="2"/>
     </font>
@@ -499,6 +489,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -520,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -643,36 +641,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -783,6 +751,93 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -791,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -804,10 +859,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -823,91 +878,106 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1246,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:Q8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K2:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1270,256 +1340,258 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="39"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="18"/>
     </row>
     <row r="3" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="41"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="27"/>
     </row>
     <row r="4" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="24"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="46"/>
     </row>
     <row r="5" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="33"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27"/>
     </row>
     <row r="6" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
     </row>
     <row r="7" spans="1:17" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="32"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="35"/>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="25"/>
-    </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="27"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="23"/>
     </row>
     <row r="9" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C9" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="13" t="s">
+      <c r="G9" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="H9" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="I9" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="13" t="s">
+      <c r="O9" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="P9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="13" t="s">
+      <c r="Q9" s="40" t="s">
         <v>20</v>
-      </c>
-      <c r="Q9" s="15" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="L10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="M10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="16"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="41"/>
     </row>
     <row r="11" spans="1:17" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
@@ -1593,7 +1665,34 @@
     <row r="26" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" ht="17" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="34">
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="B8:Q8"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:Q7"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="I2:J2"/>
@@ -1601,31 +1700,6 @@
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="B8:Q8"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="J9:M9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>